<commit_message>
Added a couple more things to the Master BOM
</commit_message>
<xml_diff>
--- a/BOM/BOM_Master_2018.xlsx
+++ b/BOM/BOM_Master_2018.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tom_Mac/Documents/GitHub/rover-hardware/BOM/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A0AFEA-6530-A044-B96F-3839CC477D65}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935" firstSheet="5" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="37780" windowHeight="21180" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Total Cost" sheetId="1" r:id="rId1"/>
@@ -20,12 +26,12 @@
     <sheet name="Antenna" sheetId="13" r:id="rId11"/>
     <sheet name="Misc" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="179021" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="197">
   <si>
     <t>Manufacturer No.</t>
   </si>
@@ -135,9 +141,6 @@
     <t>gold plated 8 awg pin</t>
   </si>
   <si>
-    <t>gold plated 4 awg pin</t>
-  </si>
-  <si>
     <t>Mouser</t>
   </si>
   <si>
@@ -247,9 +250,6 @@
   </si>
   <si>
     <t>To be installed on master elec box</t>
-  </si>
-  <si>
-    <t>4 conductor 12 AWG</t>
   </si>
   <si>
     <t>P14C-22GBK</t>
@@ -571,12 +571,87 @@
   <si>
     <t>TRINKET MINI MCU BOARD 3.3V</t>
   </si>
+  <si>
+    <t>Automotive Connectors SZ 20 STAMP CONT SKT Loose Piece</t>
+  </si>
+  <si>
+    <t>1062-20-0122</t>
+  </si>
+  <si>
+    <t>te Connectivity</t>
+  </si>
+  <si>
+    <t>CONTACT PIN 12-14AWG CRIMP TIN</t>
+  </si>
+  <si>
+    <t>1060-12-0166</t>
+  </si>
+  <si>
+    <t>CONTACT SKT 12-14AWG CRIMP TIN</t>
+  </si>
+  <si>
+    <t>for 12 AWG plug</t>
+  </si>
+  <si>
+    <t>for 12AWG receptacles</t>
+  </si>
+  <si>
+    <t>1062-12-0166</t>
+  </si>
+  <si>
+    <t>CONTACT SKT 8-10AWG CRIMP NICKEL</t>
+  </si>
+  <si>
+    <t>check cable size before ordering</t>
+  </si>
+  <si>
+    <t>0462-203-08141</t>
+  </si>
+  <si>
+    <t>gold plated 6 awg pin</t>
+  </si>
+  <si>
+    <t>CONTACT SKT 6AWG CRIMP NICKEL</t>
+  </si>
+  <si>
+    <t>0462-203-04141</t>
+  </si>
+  <si>
+    <t>for 4 awg receptacles</t>
+  </si>
+  <si>
+    <t>for 18 AWG receptacles</t>
+  </si>
+  <si>
+    <t>for Arm motors</t>
+  </si>
+  <si>
+    <t>For power</t>
+  </si>
+  <si>
+    <t>3 conductor 12 AWG</t>
+  </si>
+  <si>
+    <t>9123-150M</t>
+  </si>
+  <si>
+    <t>Modular Connectors / Ethernet Connectors ANEL MT RECEPT IDC KRONE TERMINALS</t>
+  </si>
+  <si>
+    <t>NE8FAV-YK</t>
+  </si>
+  <si>
+    <t>Cable Mounting &amp; Accessories Han CGM-P M32x1,5 D.18-25mm black</t>
+  </si>
+  <si>
+    <t>junction box made from kevlar</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -655,6 +730,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -692,7 +779,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -743,6 +830,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -753,6 +842,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -801,7 +893,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -834,9 +926,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -869,6 +978,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1044,40 +1170,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="50.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.5703125" customWidth="1"/>
-    <col min="11" max="11" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.28515625" customWidth="1"/>
-    <col min="13" max="13" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.5" customWidth="1"/>
+    <col min="11" max="11" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.33203125" customWidth="1"/>
+    <col min="13" max="13" width="14.83203125" customWidth="1"/>
     <col min="14" max="14" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30">
+    <row r="1" spans="1:4">
       <c r="B1" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>106</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B2" s="8">
         <v>2</v>
@@ -1091,7 +1217,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B3">
         <v>6</v>
@@ -1105,7 +1231,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -1119,21 +1245,21 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -1147,24 +1273,24 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B8">
         <f>B3*'Drive Motor Cables'!$J$1</f>
-        <v>254.274</v>
+        <v>242.93399999999997</v>
       </c>
       <c r="C8">
         <f>C3*'Drive Motor Cables'!$J$2</f>
-        <v>262.07399999999996</v>
+        <v>250.73399999999998</v>
       </c>
       <c r="D8">
         <f>D3*'Drive Motor Cables'!$J$3</f>
-        <v>269.87399999999997</v>
+        <v>258.53399999999993</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B9">
         <f>'Battery Power Cable'!$J$1</f>
@@ -1181,7 +1307,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B10">
         <f>'I2C Cable'!$J$1*'Total Cost'!B6</f>
@@ -1198,7 +1324,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B11">
         <f>SUM(Tools!G2:G5)</f>
@@ -1215,24 +1341,24 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B12">
         <f>B2*'Arm Box BOM'!$J$1</f>
-        <v>559.55399999999997</v>
+        <v>570.50399999999991</v>
       </c>
       <c r="C12">
         <f>C2*'Arm Box BOM'!$J$1</f>
-        <v>839.3309999999999</v>
+        <v>855.75599999999986</v>
       </c>
       <c r="D12">
         <f>D2*'Arm Box BOM'!$J$1</f>
-        <v>1119.1079999999999</v>
+        <v>1141.0079999999998</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B13">
         <f>SUM('I2C Cable'!$G3:$G4)</f>
@@ -1249,36 +1375,36 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B14">
         <f>'Master Elec Box'!$J$1</f>
-        <v>440.54</v>
+        <v>505.51</v>
       </c>
       <c r="C14">
         <f>'Master Elec Box'!$J$1</f>
-        <v>440.54</v>
+        <v>505.51</v>
       </c>
       <c r="D14">
         <f>'Master Elec Box'!$J$1</f>
-        <v>440.54</v>
+        <v>505.51</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B15">
         <f>SUM(B8:B14)</f>
-        <v>1433.3879999999999</v>
+        <v>1497.9679999999998</v>
       </c>
       <c r="C15">
         <f>SUM(C8:C14)</f>
-        <v>1769.6249999999998</v>
+        <v>1839.6799999999998</v>
       </c>
       <c r="D15">
         <f>SUM(D8:D14)</f>
-        <v>2084.732</v>
+        <v>2160.2619999999997</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -1360,19 +1486,19 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1380,7 +1506,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1398,18 +1524,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="25.5">
+    <row r="2" spans="1:7" ht="26">
       <c r="A2" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2" t="s">
         <v>152</v>
       </c>
-      <c r="C2" t="s">
-        <v>154</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -1424,7 +1550,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -1433,21 +1559,25 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="4" max="4" width="90.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1465,15 +1595,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="25.5">
+    <row r="2" spans="1:7" ht="28">
       <c r="A2" s="21" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -1482,21 +1612,78 @@
         <v>357.77</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="25.5">
+    <row r="3" spans="1:7" ht="26">
       <c r="A3" s="20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D3" t="s">
         <v>166</v>
-      </c>
-      <c r="D3" t="s">
-        <v>168</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3">
         <v>105.07</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="17">
+      <c r="A4" s="26" t="s">
+        <v>194</v>
+      </c>
+      <c r="B4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="E4">
+        <v>6</v>
+      </c>
+      <c r="F4">
+        <v>13.01</v>
+      </c>
+      <c r="G4">
+        <f>E4*F4</f>
+        <v>78.06</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="17">
+      <c r="A5" s="26">
+        <v>19000005187</v>
+      </c>
+      <c r="B5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>195</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>19.95</v>
+      </c>
+      <c r="G5">
+        <f>E5*F5</f>
+        <v>39.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="D6" t="s">
+        <v>196</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>50</v>
+      </c>
+      <c r="G6">
+        <f>E6*F6</f>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1505,16 +1692,16 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1522,7 +1709,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1542,16 +1729,16 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="B2" t="s">
         <v>161</v>
       </c>
-      <c r="B2" t="s">
-        <v>163</v>
-      </c>
       <c r="C2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -1570,17 +1757,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15:F15"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="4" max="4" width="60.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="60.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -1588,7 +1775,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1606,28 +1793,28 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="J1">
-        <f>SUM(G2:G13)</f>
-        <v>440.54</v>
+        <f>SUM(G2:G17)</f>
+        <v>505.51</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -1636,279 +1823,383 @@
         <v>13.9</v>
       </c>
       <c r="G2">
-        <f t="shared" ref="G2:G14" si="0">E2*F2</f>
+        <f t="shared" ref="G2:G18" si="0">E2*F2</f>
         <v>13.9</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
-      <c r="A3" t="s">
-        <v>23</v>
+    <row r="3" spans="1:10" ht="16">
+      <c r="A3" s="27" t="s">
+        <v>176</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" t="s">
-        <v>24</v>
+        <v>36</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>175</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F3">
-        <v>17.309999999999999</v>
+        <v>0.48</v>
       </c>
       <c r="G3">
         <f t="shared" si="0"/>
-        <v>17.309999999999999</v>
+        <v>4.8</v>
+      </c>
+      <c r="H3" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4">
-        <v>2.04</v>
+        <v>17.309999999999999</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>2.04</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" t="s">
-        <v>28</v>
+        <v>17.309999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="16">
+      <c r="A5" s="27" t="s">
+        <v>186</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>1.88</v>
-      </c>
-      <c r="G5">
-        <f t="shared" si="0"/>
-        <v>1.88</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" t="s">
-        <v>30</v>
+        <v>36</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="16">
+      <c r="A6" s="27" t="s">
+        <v>183</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" t="s">
-        <v>31</v>
+        <v>36</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>181</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F6">
-        <v>2.08</v>
+        <v>5.78</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>2.08</v>
+        <v>23.12</v>
+      </c>
+      <c r="H6" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>87</v>
+        <v>27</v>
       </c>
       <c r="E7">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F7">
-        <v>18.510000000000002</v>
+        <v>2.04</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>111.06</v>
+        <v>4.08</v>
+      </c>
+      <c r="H7" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F8">
-        <v>1.89</v>
+        <v>1.88</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>1.89</v>
+        <v>3.76</v>
+      </c>
+      <c r="H8" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>2.08</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>4.16</v>
+      </c>
+      <c r="H9" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" t="s">
+        <v>85</v>
+      </c>
+      <c r="E10">
+        <v>6</v>
+      </c>
+      <c r="F10">
+        <v>18.510000000000002</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>111.06</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11">
+        <v>54</v>
+      </c>
+      <c r="F11">
+        <v>0.4</v>
+      </c>
+      <c r="G11">
+        <f>E11*F11</f>
+        <v>21.6</v>
+      </c>
+      <c r="H11" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12">
+        <v>6</v>
+      </c>
+      <c r="F12">
+        <v>1.89</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>11.34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="B13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" t="s">
         <v>14</v>
       </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
         <v>3.84</v>
       </c>
-      <c r="G9">
+      <c r="G13">
         <f t="shared" si="0"/>
         <v>3.84</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="1">
+    <row r="14" spans="1:10">
+      <c r="A14" s="1">
         <v>4946</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E10" s="5">
+      <c r="B14" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14" s="5">
         <v>50</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F14" s="5">
         <v>0.66300000000000003</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G14" s="5">
         <f t="shared" si="0"/>
         <v>33.15</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="1">
+    <row r="15" spans="1:10">
+      <c r="A15" s="1">
         <v>3299</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E11" s="5">
-        <v>1</v>
-      </c>
-      <c r="F11" s="5">
+      <c r="B15" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E15" s="5">
+        <v>1</v>
+      </c>
+      <c r="F15" s="5">
         <v>23.39</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G15" s="5">
         <f t="shared" si="0"/>
         <v>23.39</v>
       </c>
-      <c r="H11" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="D12" t="s">
-        <v>121</v>
-      </c>
-      <c r="E12">
+      <c r="H15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="D16" t="s">
+        <v>119</v>
+      </c>
+      <c r="E16">
         <v>2</v>
       </c>
-      <c r="F12">
+      <c r="F16">
         <v>15</v>
       </c>
-      <c r="G12">
+      <c r="G16">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
-      <c r="D13" t="s">
-        <v>122</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13">
+    <row r="17" spans="1:7">
+      <c r="D17" t="s">
+        <v>120</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
         <v>200</v>
       </c>
-      <c r="G13">
+      <c r="G17">
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="B14" t="s">
-        <v>158</v>
-      </c>
-      <c r="C14" t="s">
+    <row r="18" spans="1:7">
+      <c r="A18" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B18" t="s">
+        <v>156</v>
+      </c>
+      <c r="C18" t="s">
+        <v>152</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14">
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
         <v>3.39</v>
       </c>
-      <c r="G14">
+      <c r="G18">
         <f t="shared" si="0"/>
         <v>3.39</v>
       </c>
@@ -1919,17 +2210,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="4" max="4" width="60.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="60.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -1937,7 +2228,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1955,14 +2246,14 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="J1">
-        <f>SUM(G2:G11)</f>
-        <v>279.77699999999999</v>
+        <f>SUM(G2:G12)</f>
+        <v>285.25199999999995</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -1970,13 +2261,13 @@
         <v>19000005182</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="C2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="E2">
         <v>6</v>
@@ -1985,22 +2276,22 @@
         <v>6.54</v>
       </c>
       <c r="G2">
-        <f t="shared" ref="G2:G12" si="0">E2*F2</f>
+        <f t="shared" ref="G2:G13" si="0">E2*F2</f>
         <v>39.24</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="B3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -2013,191 +2304,233 @@
         <v>11.59</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4" t="s">
-        <v>68</v>
+    <row r="4" spans="1:10" ht="16">
+      <c r="A4" s="27" t="s">
+        <v>180</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" t="s">
-        <v>69</v>
+        <v>36</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>177</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F4">
-        <v>6.89</v>
+        <v>0.77</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>6.89</v>
+        <v>4.62</v>
+      </c>
+      <c r="H4" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>6.89</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>6.89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
+      <c r="B6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
         <v>2.75</v>
       </c>
-      <c r="G5">
+      <c r="G6">
         <f t="shared" si="0"/>
         <v>2.75</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
-      <c r="A6">
+    <row r="7" spans="1:10">
+      <c r="A7">
         <v>114017</v>
       </c>
-      <c r="B6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" t="s">
         <v>16</v>
-      </c>
-      <c r="E6">
-        <v>3</v>
-      </c>
-      <c r="F6">
-        <v>0.34499999999999997</v>
-      </c>
-      <c r="G6">
-        <f t="shared" si="0"/>
-        <v>1.0349999999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" t="s">
-        <v>70</v>
       </c>
       <c r="E7">
         <v>6</v>
       </c>
       <c r="F7">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="H7" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8">
+        <v>6</v>
+      </c>
+      <c r="F8">
         <v>0.66200000000000003</v>
       </c>
-      <c r="G7">
+      <c r="G8">
         <f t="shared" si="0"/>
         <v>3.9720000000000004</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="16.5">
-      <c r="A8" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B8" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" t="s">
-        <v>76</v>
-      </c>
-      <c r="E8">
-        <v>30</v>
-      </c>
-      <c r="F8">
-        <v>1.61</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="0"/>
-        <v>48.300000000000004</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" ht="17">
+      <c r="A9" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" t="s">
+        <v>59</v>
+      </c>
       <c r="D9" t="s">
         <v>74</v>
       </c>
       <c r="E9">
+        <v>30</v>
+      </c>
+      <c r="F9">
+        <v>1.61</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>48.300000000000004</v>
+      </c>
+      <c r="H9" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
+        <v>192</v>
+      </c>
+      <c r="B10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" t="s">
+        <v>191</v>
+      </c>
+      <c r="E10">
         <v>3</v>
       </c>
-      <c r="F9">
-        <v>2</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="D10" t="s">
-        <v>121</v>
-      </c>
-      <c r="E10">
-        <v>2</v>
-      </c>
       <c r="F10">
-        <v>10</v>
+        <v>1.94</v>
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>5.82</v>
+      </c>
+      <c r="H10" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="D11" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F11">
+        <v>10</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="D12" t="s">
+        <v>120</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
         <v>140</v>
       </c>
-      <c r="G11">
+      <c r="G12">
         <f t="shared" si="0"/>
         <v>140</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12">
+    <row r="13" spans="1:10">
+      <c r="A13" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
         <v>5.81</v>
       </c>
-      <c r="G12">
+      <c r="G13">
         <f t="shared" si="0"/>
         <v>5.81</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
-      <c r="D13" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="E13">
+    <row r="14" spans="1:10">
+      <c r="D14" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E14">
         <v>40</v>
       </c>
     </row>
@@ -2207,19 +2540,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="47.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -2227,7 +2560,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -2245,124 +2578,124 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="J1">
         <f>SUM(G2:G7,G14:G17)</f>
-        <v>42.378999999999998</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="13" t="s">
-        <v>6</v>
+        <v>40.488999999999997</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="17">
+      <c r="A2" s="26" t="s">
+        <v>173</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>174</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" t="s">
-        <v>86</v>
+        <v>89</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>172</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F2">
-        <v>17.61</v>
+        <v>0.59</v>
       </c>
       <c r="G2">
-        <f t="shared" ref="G2:G9" si="0">E2*F2</f>
-        <v>17.61</v>
+        <f>E2*F2</f>
+        <v>5.31</v>
       </c>
       <c r="I2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="J2">
         <f>SUM(G2:G6,G8,G14:G17)</f>
-        <v>43.678999999999995</v>
+        <v>41.788999999999994</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="13" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>84</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3">
-        <v>6.89</v>
+        <v>17.61</v>
       </c>
       <c r="G3">
-        <f t="shared" si="0"/>
-        <v>6.89</v>
+        <f>E3*F3</f>
+        <v>17.61</v>
       </c>
       <c r="I3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="J3">
         <f>SUM(G2:G6,G9,G14:G17)</f>
-        <v>44.978999999999992</v>
+        <v>43.088999999999992</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4">
-        <v>2.75</v>
+        <v>6.89</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
-        <v>2.75</v>
+        <f>E4*F4</f>
+        <v>6.89</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E5">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="F5">
-        <v>0.4</v>
+        <v>2.75</v>
       </c>
       <c r="G5">
-        <f t="shared" si="0"/>
-        <v>7.2</v>
+        <f>E5*F5</f>
+        <v>2.75</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -2370,10 +2703,10 @@
         <v>114017</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s">
         <v>16</v>
@@ -2385,19 +2718,19 @@
         <v>0.34499999999999997</v>
       </c>
       <c r="G6">
-        <f t="shared" si="0"/>
+        <f>E6*F6</f>
         <v>1.0349999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="16.5">
+    <row r="7" spans="1:10" ht="17">
       <c r="A7" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" t="s">
         <v>59</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
         <v>60</v>
-      </c>
-      <c r="D7" t="s">
-        <v>61</v>
       </c>
       <c r="E7">
         <f>'Total Cost'!B4</f>
@@ -2407,22 +2740,22 @@
         <v>1.3</v>
       </c>
       <c r="G7">
-        <f t="shared" si="0"/>
+        <f>E7*F7</f>
         <v>5.2</v>
       </c>
       <c r="H7" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="16.5">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="17">
       <c r="A8" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" t="s">
         <v>59</v>
       </c>
-      <c r="B8" t="s">
+      <c r="D8" t="s">
         <v>60</v>
-      </c>
-      <c r="D8" t="s">
-        <v>61</v>
       </c>
       <c r="E8">
         <f>'Total Cost'!C4</f>
@@ -2432,22 +2765,22 @@
         <v>1.3</v>
       </c>
       <c r="G8">
-        <f t="shared" si="0"/>
+        <f>E8*F8</f>
         <v>6.5</v>
       </c>
       <c r="H8" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="16.5">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="17">
       <c r="A9" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" t="s">
         <v>59</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D9" t="s">
         <v>60</v>
-      </c>
-      <c r="D9" t="s">
-        <v>61</v>
       </c>
       <c r="E9">
         <f>'Total Cost'!D4</f>
@@ -2457,32 +2790,32 @@
         <v>1.3</v>
       </c>
       <c r="G9">
-        <f t="shared" si="0"/>
+        <f>E9*F9</f>
         <v>7.8000000000000007</v>
       </c>
       <c r="H9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="15"/>
       <c r="D12" s="10"/>
     </row>
-    <row r="13" spans="1:10" ht="16.5">
+    <row r="13" spans="1:10" ht="17">
       <c r="A13" s="14" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="45">
       <c r="A14" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>144</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>146</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="19" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E14" s="5">
         <v>1</v>
@@ -2491,7 +2824,7 @@
         <v>0.48</v>
       </c>
       <c r="G14" s="16">
-        <f t="shared" ref="G14:G17" si="1">E14*F14</f>
+        <f t="shared" ref="G14:G17" si="0">E14*F14</f>
         <v>0.48</v>
       </c>
       <c r="H14" s="5"/>
@@ -2503,11 +2836,11 @@
         <v>2061131</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E15" s="5">
         <v>6</v>
@@ -2516,25 +2849,25 @@
         <v>5.7000000000000002E-2</v>
       </c>
       <c r="G15" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.34200000000000003</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" spans="1:10" ht="45">
+    <row r="16" spans="1:10" ht="30">
       <c r="A16" s="18" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="19" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E16" s="5">
         <v>1</v>
@@ -2543,7 +2876,7 @@
         <v>0.5</v>
       </c>
       <c r="G16" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="H16" s="5"/>
@@ -2555,11 +2888,11 @@
         <v>2062101</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E17" s="5">
         <v>6</v>
@@ -2568,42 +2901,42 @@
         <v>6.2E-2</v>
       </c>
       <c r="G17" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.372</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:10">
       <c r="D18" s="12" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A15" r:id="rId1" display="https://www.molex.com/molex/products/datasheet.jsp?part=active/0002061131_CRIMP_TERMINALS.xml"/>
-    <hyperlink ref="A17" r:id="rId2" display="https://www.molex.com/molex/products/datasheet.jsp?part=active/0002062101_CRIMP_TERMINALS.xml"/>
+    <hyperlink ref="A15" r:id="rId1" display="https://www.molex.com/molex/products/datasheet.jsp?part=active/0002061131_CRIMP_TERMINALS.xml" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="A17" r:id="rId2" display="https://www.molex.com/molex/products/datasheet.jsp?part=active/0002062101_CRIMP_TERMINALS.xml" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="50.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -2611,7 +2944,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -2629,7 +2962,7 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I1" t="s">
         <v>5</v>
@@ -2644,10 +2977,10 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
         <v>18</v>
@@ -2668,10 +3001,10 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
         <v>20</v>
@@ -2692,10 +3025,10 @@
         <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
         <v>22</v>
@@ -2713,13 +3046,13 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
         <v>25</v>
@@ -2737,13 +3070,13 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s">
         <v>35</v>
@@ -2761,16 +3094,16 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>184</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -2789,17 +3122,17 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -2807,7 +3140,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -2825,10 +3158,10 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="J1">
         <f>SUM(G2:G5)</f>
@@ -2840,10 +3173,10 @@
         <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
         <v>33</v>
@@ -2859,7 +3192,7 @@
         <v>2.19</v>
       </c>
       <c r="I2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="J2">
         <f>SUM(G2:G6)</f>
@@ -2871,10 +3204,10 @@
         <v>114008</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
         <v>33</v>
@@ -2895,10 +3228,10 @@
         <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
         <v>33</v>
@@ -2919,13 +3252,13 @@
         <v>422</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>92</v>
       </c>
       <c r="E5" s="5">
         <v>2</v>
@@ -2943,13 +3276,13 @@
         <v>3445</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>91</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>93</v>
       </c>
       <c r="E6" s="5">
         <v>1</v>
@@ -2962,21 +3295,21 @@
         <v>27.53</v>
       </c>
       <c r="H6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>124</v>
-      </c>
-      <c r="B7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" t="s">
-        <v>125</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>126</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -2989,21 +3322,21 @@
         <v>122.2</v>
       </c>
       <c r="H7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D8" s="10" t="s">
         <v>125</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>127</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -3016,12 +3349,12 @@
         <v>51.51</v>
       </c>
       <c r="H8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A6" r:id="rId1" display="https://www.mouser.ca/ProductDetail/Adafruit/3445?qs=sGAEpiMZZMu%252bmKbOcEVhFQxTf6VNDqZlHHxJgTmlxQIH1iVmUF7%252bAg%3d%3d"/>
+    <hyperlink ref="A6" r:id="rId1" display="https://www.mouser.ca/ProductDetail/Adafruit/3445?qs=sGAEpiMZZMu%252bmKbOcEVhFQxTf6VNDqZlHHxJgTmlxQIH1iVmUF7%252bAg%3d%3d" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="17" orientation="portrait" verticalDpi="0" r:id="rId2"/>
@@ -3029,27 +3362,27 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8:G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="79.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="79.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="J1" s="5">
         <f>SUM(G6:G7)</f>
@@ -3061,7 +3394,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -3081,16 +3414,16 @@
     </row>
     <row r="3" spans="1:10" ht="30">
       <c r="A3" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E3" s="5">
         <v>2</v>
@@ -3103,21 +3436,21 @@
         <v>13.66</v>
       </c>
       <c r="H3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E4" s="5">
         <v>2</v>
@@ -3132,16 +3465,16 @@
     </row>
     <row r="6" spans="1:10" ht="30">
       <c r="A6" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>84</v>
       </c>
       <c r="E6" s="5">
         <v>1</v>
@@ -3156,16 +3489,16 @@
     </row>
     <row r="7" spans="1:10" ht="30">
       <c r="A7" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E7" s="5">
         <v>1</v>
@@ -3191,21 +3524,21 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="A10:C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="79.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="79.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -3213,7 +3546,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -3231,21 +3564,21 @@
         <v>5</v>
       </c>
       <c r="H2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -3260,16 +3593,16 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -3284,16 +3617,16 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -3308,16 +3641,16 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -3330,18 +3663,18 @@
         <v>3.49</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1">
+    <row r="8" spans="1:8" ht="16" thickBot="1">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -3359,13 +3692,13 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" t="s">
         <v>43</v>
-      </c>
-      <c r="B12" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" t="s">
-        <v>44</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -3378,7 +3711,7 @@
         <v>8.49</v>
       </c>
       <c r="H12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -3388,16 +3721,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="56.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -3405,10 +3738,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -3431,14 +3764,14 @@
         <v>1386</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F3" s="5">
         <v>1</v>
@@ -3447,25 +3780,25 @@
         <v>49.61</v>
       </c>
       <c r="H3" s="5">
-        <f>F3*G3</f>
+        <f t="shared" ref="H3:H8" si="0">F3*G3</f>
         <v>49.61</v>
       </c>
       <c r="I3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="25.5">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="26">
       <c r="A4" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="B4" t="s">
-        <v>132</v>
-      </c>
-      <c r="D4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>133</v>
       </c>
       <c r="F4" s="5">
         <v>3</v>
@@ -3474,26 +3807,26 @@
         <v>15.48</v>
       </c>
       <c r="H4" s="5">
-        <f>F4*G4</f>
+        <f t="shared" si="0"/>
         <v>46.44</v>
       </c>
       <c r="I4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="25.5">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="26">
       <c r="A5" s="22" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="23" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F5" s="23">
         <v>1</v>
@@ -3502,25 +3835,25 @@
         <v>20.66</v>
       </c>
       <c r="H5" s="25">
-        <f>F5*G5</f>
+        <f t="shared" si="0"/>
         <v>20.66</v>
       </c>
       <c r="I5" s="23" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="26">
+      <c r="A6" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B6" t="s">
+        <v>130</v>
+      </c>
+      <c r="D6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>137</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="25.5">
-      <c r="A6" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B6" t="s">
-        <v>132</v>
-      </c>
-      <c r="D6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>139</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -3529,7 +3862,7 @@
         <v>15.48</v>
       </c>
       <c r="H6" s="5">
-        <f>F6*G6</f>
+        <f t="shared" si="0"/>
         <v>15.48</v>
       </c>
     </row>
@@ -3538,13 +3871,13 @@
         <v>3317</v>
       </c>
       <c r="B7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -3553,7 +3886,7 @@
         <v>21.93</v>
       </c>
       <c r="H7" s="5">
-        <f>F7*G7</f>
+        <f t="shared" si="0"/>
         <v>21.93</v>
       </c>
     </row>
@@ -3562,16 +3895,16 @@
         <v>1500</v>
       </c>
       <c r="B8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -3580,7 +3913,7 @@
         <v>9.76</v>
       </c>
       <c r="H8" s="5">
-        <f>F8*G8</f>
+        <f t="shared" si="0"/>
         <v>9.76</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added a couple lines to the USB sheet
</commit_message>
<xml_diff>
--- a/BOM/BOM_Master_2018.xlsx
+++ b/BOM/BOM_Master_2018.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10709"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tom_Mac/Documents/GitHub/rover-hardware/BOM/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A0AFEA-6530-A044-B96F-3839CC477D65}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="37780" windowHeight="21180" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="37785" windowHeight="15990" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Total Cost" sheetId="1" r:id="rId1"/>
@@ -20,18 +14,19 @@
     <sheet name="Battery Power Cable" sheetId="3" r:id="rId5"/>
     <sheet name="Tools" sheetId="4" r:id="rId6"/>
     <sheet name="I2C Cable" sheetId="7" r:id="rId7"/>
-    <sheet name="CAN BUS Cable" sheetId="9" r:id="rId8"/>
-    <sheet name="Potential Arm Stuff" sheetId="8" r:id="rId9"/>
-    <sheet name="Power Board BOM" sheetId="11" r:id="rId10"/>
-    <sheet name="Antenna" sheetId="13" r:id="rId11"/>
-    <sheet name="Misc" sheetId="12" r:id="rId12"/>
+    <sheet name="USB Cable" sheetId="14" r:id="rId8"/>
+    <sheet name="CAN BUS Cable" sheetId="9" r:id="rId9"/>
+    <sheet name="Potential Arm Stuff" sheetId="8" r:id="rId10"/>
+    <sheet name="Power Board BOM" sheetId="11" r:id="rId11"/>
+    <sheet name="Antenna" sheetId="13" r:id="rId12"/>
+    <sheet name="Misc" sheetId="12" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="179021" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="203">
   <si>
     <t>Manufacturer No.</t>
   </si>
@@ -646,11 +641,29 @@
   <si>
     <t>junction box made from kevlar</t>
   </si>
+  <si>
+    <t>For USB communication</t>
+  </si>
+  <si>
+    <t>MUSBR-AHD2-241SK</t>
+  </si>
+  <si>
+    <t>Amphenol</t>
+  </si>
+  <si>
+    <t>USB Connectors IP67 Boot Style Hood Black for plug side</t>
+  </si>
+  <si>
+    <t>USB Connectors Rugged USB 3.0 A Vert Standard Shell</t>
+  </si>
+  <si>
+    <t>MUSBR-3593-M0</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="14">
     <font>
       <sz val="11"/>
@@ -893,7 +906,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -926,26 +939,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -978,23 +974,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1170,27 +1149,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="50.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.5" customWidth="1"/>
-    <col min="11" max="11" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.33203125" customWidth="1"/>
-    <col min="13" max="13" width="14.83203125" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.42578125" customWidth="1"/>
+    <col min="11" max="11" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.28515625" customWidth="1"/>
+    <col min="13" max="13" width="14.85546875" customWidth="1"/>
     <col min="14" max="14" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" ht="30">
       <c r="B1" s="8" t="s">
         <v>104</v>
       </c>
@@ -1486,19 +1465,221 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <cols>
+    <col min="5" max="5" width="56.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="1">
+        <v>1386</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" s="5">
+        <v>1</v>
+      </c>
+      <c r="G3" s="5">
+        <v>49.61</v>
+      </c>
+      <c r="H3" s="5">
+        <f t="shared" ref="H3:H8" si="0">F3*G3</f>
+        <v>49.61</v>
+      </c>
+      <c r="I3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="25.5">
+      <c r="A4" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F4" s="5">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>15.48</v>
+      </c>
+      <c r="H4" s="5">
+        <f t="shared" si="0"/>
+        <v>46.44</v>
+      </c>
+      <c r="I4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="25.5">
+      <c r="A5" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="F5" s="23">
+        <v>1</v>
+      </c>
+      <c r="G5" s="23">
+        <v>20.66</v>
+      </c>
+      <c r="H5" s="25">
+        <f t="shared" si="0"/>
+        <v>20.66</v>
+      </c>
+      <c r="I5" s="23" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="25.5">
+      <c r="A6" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B6" t="s">
+        <v>130</v>
+      </c>
+      <c r="D6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>15.48</v>
+      </c>
+      <c r="H6" s="5">
+        <f t="shared" si="0"/>
+        <v>15.48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="1">
+        <v>3317</v>
+      </c>
+      <c r="B7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>21.93</v>
+      </c>
+      <c r="H7" s="5">
+        <f t="shared" si="0"/>
+        <v>21.93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8">
+        <v>1500</v>
+      </c>
+      <c r="B8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="D8" t="s">
+        <v>123</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>9.76</v>
+      </c>
+      <c r="H8" s="5">
+        <f t="shared" si="0"/>
+        <v>9.76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1524,7 +1705,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="26">
+    <row r="2" spans="1:7" ht="25.5">
       <c r="A2" s="1" t="s">
         <v>151</v>
       </c>
@@ -1551,139 +1732,6 @@
     <row r="3" spans="1:7">
       <c r="D3" t="s">
         <v>153</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:G6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="4" max="4" width="90.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="28">
-      <c r="A2" s="21" t="s">
-        <v>165</v>
-      </c>
-      <c r="B2" t="s">
-        <v>164</v>
-      </c>
-      <c r="D2" t="s">
-        <v>163</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>357.77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="26">
-      <c r="A3" s="20" t="s">
-        <v>167</v>
-      </c>
-      <c r="B3" t="s">
-        <v>164</v>
-      </c>
-      <c r="D3" t="s">
-        <v>166</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>105.07</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="17">
-      <c r="A4" s="26" t="s">
-        <v>194</v>
-      </c>
-      <c r="B4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D4" s="26" t="s">
-        <v>193</v>
-      </c>
-      <c r="E4">
-        <v>6</v>
-      </c>
-      <c r="F4">
-        <v>13.01</v>
-      </c>
-      <c r="G4">
-        <f>E4*F4</f>
-        <v>78.06</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="17">
-      <c r="A5" s="26">
-        <v>19000005187</v>
-      </c>
-      <c r="B5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D5" s="26" t="s">
-        <v>195</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="F5">
-        <v>19.95</v>
-      </c>
-      <c r="G5">
-        <f>E5*F5</f>
-        <v>39.9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="D6" t="s">
-        <v>196</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="F6">
-        <v>50</v>
-      </c>
-      <c r="G6">
-        <f>E6*F6</f>
-        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1692,16 +1740,149 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="90.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="B2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>357.77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="B3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D3" t="s">
+        <v>166</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>105.07</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="16.5">
+      <c r="A4" s="26" t="s">
+        <v>194</v>
+      </c>
+      <c r="B4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="E4">
+        <v>6</v>
+      </c>
+      <c r="F4">
+        <v>13.01</v>
+      </c>
+      <c r="G4">
+        <f>E4*F4</f>
+        <v>78.06</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="16.5">
+      <c r="A5" s="26">
+        <v>19000005187</v>
+      </c>
+      <c r="B5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>195</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>19.95</v>
+      </c>
+      <c r="G5">
+        <f>E5*F5</f>
+        <v>39.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="D6" t="s">
+        <v>196</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>50</v>
+      </c>
+      <c r="G6">
+        <f>E6*F6</f>
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1757,17 +1938,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="4" max="4" width="60.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="60.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -1827,7 +2008,7 @@
         <v>13.9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="16">
+    <row r="3" spans="1:10" ht="15.75">
       <c r="A3" s="27" t="s">
         <v>176</v>
       </c>
@@ -1878,7 +2059,7 @@
         <v>17.309999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="16">
+    <row r="5" spans="1:10" ht="15.75">
       <c r="A5" s="27" t="s">
         <v>186</v>
       </c>
@@ -1892,7 +2073,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="16">
+    <row r="6" spans="1:10" ht="15.75">
       <c r="A6" s="27" t="s">
         <v>183</v>
       </c>
@@ -2210,17 +2391,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="4" max="4" width="60.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="60.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -2304,7 +2485,7 @@
         <v>11.59</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="16">
+    <row r="4" spans="1:10" ht="15.75">
       <c r="A4" s="27" t="s">
         <v>180</v>
       </c>
@@ -2430,7 +2611,7 @@
         <v>3.9720000000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="17">
+    <row r="9" spans="1:10" ht="16.5">
       <c r="A9" s="3" t="s">
         <v>73</v>
       </c>
@@ -2540,19 +2721,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="47.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -2588,7 +2769,7 @@
         <v>40.488999999999997</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="17">
+    <row r="2" spans="1:10" ht="16.5">
       <c r="A2" s="26" t="s">
         <v>173</v>
       </c>
@@ -2608,7 +2789,7 @@
         <v>0.59</v>
       </c>
       <c r="G2">
-        <f>E2*F2</f>
+        <f t="shared" ref="G2:G9" si="0">E2*F2</f>
         <v>5.31</v>
       </c>
       <c r="I2" t="s">
@@ -2639,7 +2820,7 @@
         <v>17.61</v>
       </c>
       <c r="G3">
-        <f>E3*F3</f>
+        <f t="shared" si="0"/>
         <v>17.61</v>
       </c>
       <c r="I3" t="s">
@@ -2670,7 +2851,7 @@
         <v>6.89</v>
       </c>
       <c r="G4">
-        <f>E4*F4</f>
+        <f t="shared" si="0"/>
         <v>6.89</v>
       </c>
     </row>
@@ -2694,7 +2875,7 @@
         <v>2.75</v>
       </c>
       <c r="G5">
-        <f>E5*F5</f>
+        <f t="shared" si="0"/>
         <v>2.75</v>
       </c>
     </row>
@@ -2718,11 +2899,11 @@
         <v>0.34499999999999997</v>
       </c>
       <c r="G6">
-        <f>E6*F6</f>
+        <f t="shared" si="0"/>
         <v>1.0349999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="17">
+    <row r="7" spans="1:10" ht="16.5">
       <c r="A7" s="14" t="s">
         <v>58</v>
       </c>
@@ -2740,14 +2921,14 @@
         <v>1.3</v>
       </c>
       <c r="G7">
-        <f>E7*F7</f>
+        <f t="shared" si="0"/>
         <v>5.2</v>
       </c>
       <c r="H7" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="17">
+    <row r="8" spans="1:10" ht="16.5">
       <c r="A8" s="14" t="s">
         <v>58</v>
       </c>
@@ -2765,14 +2946,14 @@
         <v>1.3</v>
       </c>
       <c r="G8">
-        <f>E8*F8</f>
+        <f t="shared" si="0"/>
         <v>6.5</v>
       </c>
       <c r="H8" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="17">
+    <row r="9" spans="1:10" ht="16.5">
       <c r="A9" s="14" t="s">
         <v>58</v>
       </c>
@@ -2790,7 +2971,7 @@
         <v>1.3</v>
       </c>
       <c r="G9">
-        <f>E9*F9</f>
+        <f t="shared" si="0"/>
         <v>7.8000000000000007</v>
       </c>
       <c r="H9" t="s">
@@ -2801,7 +2982,7 @@
       <c r="A12" s="15"/>
       <c r="D12" s="10"/>
     </row>
-    <row r="13" spans="1:10" ht="17">
+    <row r="13" spans="1:10" ht="16.5">
       <c r="A13" s="14" t="s">
         <v>138</v>
       </c>
@@ -2824,7 +3005,7 @@
         <v>0.48</v>
       </c>
       <c r="G14" s="16">
-        <f t="shared" ref="G14:G17" si="0">E14*F14</f>
+        <f t="shared" ref="G14:G17" si="1">E14*F14</f>
         <v>0.48</v>
       </c>
       <c r="H14" s="5"/>
@@ -2849,7 +3030,7 @@
         <v>5.7000000000000002E-2</v>
       </c>
       <c r="G15" s="16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.34200000000000003</v>
       </c>
       <c r="H15" s="5" t="s">
@@ -2858,7 +3039,7 @@
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" spans="1:10" ht="30">
+    <row r="16" spans="1:10" ht="45">
       <c r="A16" s="18" t="s">
         <v>146</v>
       </c>
@@ -2876,7 +3057,7 @@
         <v>0.5</v>
       </c>
       <c r="G16" s="16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="H16" s="5"/>
@@ -2901,7 +3082,7 @@
         <v>6.2E-2</v>
       </c>
       <c r="G17" s="16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.372</v>
       </c>
       <c r="H17" s="5" t="s">
@@ -2917,26 +3098,26 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A15" r:id="rId1" display="https://www.molex.com/molex/products/datasheet.jsp?part=active/0002061131_CRIMP_TERMINALS.xml" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="A17" r:id="rId2" display="https://www.molex.com/molex/products/datasheet.jsp?part=active/0002062101_CRIMP_TERMINALS.xml" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="A15" r:id="rId1" display="https://www.molex.com/molex/products/datasheet.jsp?part=active/0002061131_CRIMP_TERMINALS.xml"/>
+    <hyperlink ref="A17" r:id="rId2" display="https://www.molex.com/molex/products/datasheet.jsp?part=active/0002062101_CRIMP_TERMINALS.xml"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="50.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -3122,17 +3303,17 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -3354,7 +3535,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A6" r:id="rId1" display="https://www.mouser.ca/ProductDetail/Adafruit/3445?qs=sGAEpiMZZMu%252bmKbOcEVhFQxTf6VNDqZlHHxJgTmlxQIH1iVmUF7%252bAg%3d%3d" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="A6" r:id="rId1" display="https://www.mouser.ca/ProductDetail/Adafruit/3445?qs=sGAEpiMZZMu%252bmKbOcEVhFQxTf6VNDqZlHHxJgTmlxQIH1iVmUF7%252bAg%3d%3d"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="17" orientation="portrait" verticalDpi="0" r:id="rId2"/>
@@ -3362,16 +3543,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8:G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="79.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="79.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -3524,21 +3705,21 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:H12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="A10:C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="79.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="79.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>102</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -3567,152 +3748,57 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="s">
-        <v>45</v>
+    <row r="3" spans="1:8" ht="38.25">
+      <c r="A3" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>12.82</v>
+      </c>
+      <c r="G3">
+        <f>F3*E3</f>
+        <v>12.82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="25.5">
+      <c r="A4" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>199</v>
       </c>
       <c r="C4" t="s">
         <v>36</v>
       </c>
-      <c r="D4" t="s">
-        <v>44</v>
+      <c r="D4" s="2" t="s">
+        <v>201</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4">
-        <v>12.31</v>
+        <v>15.07</v>
       </c>
       <c r="G4">
-        <f>E4*F4</f>
-        <v>12.31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5">
-        <v>3</v>
-      </c>
-      <c r="F5">
-        <v>0.64900000000000002</v>
-      </c>
-      <c r="G5">
-        <f>E5*F5</f>
-        <v>1.9470000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>4.62</v>
-      </c>
-      <c r="G6">
-        <f>E6*F6</f>
-        <v>4.62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" t="s">
-        <v>49</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>3.49</v>
-      </c>
-      <c r="G7">
-        <f>E7*F7</f>
-        <v>3.49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="16" thickBot="1">
-      <c r="A8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>0.248</v>
-      </c>
-      <c r="G8">
-        <f>E8*F8</f>
-        <v>0.248</v>
-      </c>
-    </row>
+        <f>F4*E4</f>
+        <v>15.07</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" thickBot="1"/>
     <row r="9" spans="1:8">
       <c r="A9" s="11"/>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B12" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <v>8.49</v>
-      </c>
-      <c r="G12">
-        <f>E12*F12</f>
-        <v>8.49</v>
-      </c>
-      <c r="H12" t="s">
-        <v>72</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3721,203 +3807,198 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:I8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="A10:C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="56.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="79.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>54</v>
       </c>
-      <c r="C1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="E2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="F2" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="G2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="1">
-        <v>1386</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="F3" s="5">
-        <v>1</v>
-      </c>
-      <c r="G3" s="5">
-        <v>49.61</v>
-      </c>
-      <c r="H3" s="5">
-        <f t="shared" ref="H3:H8" si="0">F3*G3</f>
-        <v>49.61</v>
-      </c>
-      <c r="I3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="26">
-      <c r="A4" s="1" t="s">
-        <v>129</v>
+      <c r="H2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>130</v>
+        <v>55</v>
+      </c>
+      <c r="C4" t="s">
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="F4" s="5">
+        <v>44</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>12.31</v>
+      </c>
+      <c r="G4">
+        <f>E4*F4</f>
+        <v>12.31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5">
         <v>3</v>
       </c>
-      <c r="G4">
-        <v>15.48</v>
-      </c>
-      <c r="H4" s="5">
-        <f t="shared" si="0"/>
-        <v>46.44</v>
-      </c>
-      <c r="I4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="26">
-      <c r="A5" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="E5" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="F5" s="23">
-        <v>1</v>
-      </c>
-      <c r="G5" s="23">
-        <v>20.66</v>
-      </c>
-      <c r="H5" s="25">
-        <f t="shared" si="0"/>
-        <v>20.66</v>
-      </c>
-      <c r="I5" s="23" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="26">
-      <c r="A6" s="1" t="s">
-        <v>136</v>
+      <c r="F5">
+        <v>0.64900000000000002</v>
+      </c>
+      <c r="G5">
+        <f>E5*F5</f>
+        <v>1.9470000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>130</v>
+        <v>55</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
       </c>
       <c r="D6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>137</v>
+        <v>48</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>4.62</v>
       </c>
       <c r="G6">
-        <v>15.48</v>
-      </c>
-      <c r="H6" s="5">
-        <f t="shared" si="0"/>
-        <v>15.48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="1">
-        <v>3317</v>
+        <f>E6*F6</f>
+        <v>4.62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>88</v>
+        <v>55</v>
+      </c>
+      <c r="C7" t="s">
+        <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>89</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>168</v>
+        <v>49</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>3.49</v>
       </c>
       <c r="G7">
-        <v>21.93</v>
-      </c>
-      <c r="H7" s="5">
-        <f t="shared" si="0"/>
-        <v>21.93</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8">
-        <v>1500</v>
+        <f>E7*F7</f>
+        <v>3.49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A8" t="s">
+        <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>88</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>170</v>
+        <v>55</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>123</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>171</v>
+        <v>50</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>0.248</v>
       </c>
       <c r="G8">
-        <v>9.76</v>
-      </c>
-      <c r="H8" s="5">
-        <f t="shared" si="0"/>
-        <v>9.76</v>
+        <f>E8*F8</f>
+        <v>0.248</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="11"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>8.49</v>
+      </c>
+      <c r="G12">
+        <f>E12*F12</f>
+        <v>8.49</v>
+      </c>
+      <c r="H12" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="17" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added a connector and crimper
</commit_message>
<xml_diff>
--- a/BOM/BOM_Master_2018.xlsx
+++ b/BOM/BOM_Master_2018.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="37785" windowHeight="15990" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="525" windowWidth="37785" windowHeight="15930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Total Cost" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="227">
   <si>
     <t>Manufacturer No.</t>
   </si>
@@ -659,12 +659,84 @@
   <si>
     <t>MUSBR-3593-M0</t>
   </si>
+  <si>
+    <t>left side door mount</t>
+  </si>
+  <si>
+    <t>right side door mount</t>
+  </si>
+  <si>
+    <t>2069N17</t>
+  </si>
+  <si>
+    <t>2069N15</t>
+  </si>
+  <si>
+    <t>McMaster-Carr</t>
+  </si>
+  <si>
+    <t>These would be perfect for box removal</t>
+  </si>
+  <si>
+    <t>Remote Release Latches</t>
+  </si>
+  <si>
+    <t>3985A42</t>
+  </si>
+  <si>
+    <t>1766A4</t>
+  </si>
+  <si>
+    <t>Screw on, Nickel-Plated Steel, 3-5/16" Long x 1-3/4" Wide</t>
+  </si>
+  <si>
+    <t>Come in packs of 5</t>
+  </si>
+  <si>
+    <t>EV2400</t>
+  </si>
+  <si>
+    <t>EVM Interface Board: communicate to I2C, SMBus through usb</t>
+  </si>
+  <si>
+    <t>Texas Instruments</t>
+  </si>
+  <si>
+    <t>45750-3112</t>
+  </si>
+  <si>
+    <t>Mini-Fit Plus Crimp Terminal, 16 AWG, Bag, Copper (Cu) Alloy, Tin (Sn)</t>
+  </si>
+  <si>
+    <t>from MCU to BMS board</t>
+  </si>
+  <si>
+    <t>Mini-Fit Jr. Receptacle Housing, Single Row, 3 Circuits, UL 94V-2, Natural</t>
+  </si>
+  <si>
+    <t>39-01-4030</t>
+  </si>
+  <si>
+    <t>46014-0304</t>
+  </si>
+  <si>
+    <t>Mini-Fit Plus Header, 4.20mm Pitch, Single Row, Vertical, 3 Circuits, with Snap-in Plastic Peg PCB Lock, PA Polyamide Nylon 6/6, UL 94V-0, Tin (Sn) Over Nickel (Ni) Plating</t>
+  </si>
+  <si>
+    <t>TEMCO CRIMPER &amp; CUTTER TOOL SET TH0018</t>
+  </si>
+  <si>
+    <t>TH0018</t>
+  </si>
+  <si>
+    <t>TemCo Industrial</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -755,6 +827,32 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF336633"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFEA1B39"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF707070"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -792,7 +890,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -845,6 +943,18 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1939,10 +2049,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2004,7 +2114,7 @@
         <v>13.9</v>
       </c>
       <c r="G2">
-        <f t="shared" ref="G2:G18" si="0">E2*F2</f>
+        <f t="shared" ref="G2:G19" si="0">E2*F2</f>
         <v>13.9</v>
       </c>
     </row>
@@ -2346,7 +2456,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:8">
       <c r="D17" t="s">
         <v>120</v>
       </c>
@@ -2361,7 +2471,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
         <v>155</v>
       </c>
@@ -2385,8 +2495,160 @@
         <v>3.39</v>
       </c>
     </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>205</v>
+      </c>
+      <c r="B19" t="s">
+        <v>207</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>70</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="H19" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>206</v>
+      </c>
+      <c r="B20" t="s">
+        <v>207</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>70</v>
+      </c>
+      <c r="G20">
+        <f t="shared" ref="G20:G24" si="1">E20*F20</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" t="s">
+        <v>210</v>
+      </c>
+      <c r="B21" t="s">
+        <v>207</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>88.84</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="1"/>
+        <v>88.84</v>
+      </c>
+      <c r="H21" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" t="s">
+        <v>211</v>
+      </c>
+      <c r="B22" t="s">
+        <v>207</v>
+      </c>
+      <c r="D22" s="28" t="s">
+        <v>212</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>2</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="H22" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="1"/>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="1:8" ht="22.5">
+      <c r="A24" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="D24" s="30" t="s">
+        <v>218</v>
+      </c>
+      <c r="E24">
+        <v>18</v>
+      </c>
+      <c r="H24" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="22.5">
+      <c r="A25" s="29" t="s">
+        <v>221</v>
+      </c>
+      <c r="D25" s="30" t="s">
+        <v>220</v>
+      </c>
+      <c r="E25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="33.75">
+      <c r="A26" s="29" t="s">
+        <v>222</v>
+      </c>
+      <c r="D26" s="30" t="s">
+        <v>223</v>
+      </c>
+      <c r="E26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="31" t="s">
+        <v>225</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="C27" s="16"/>
+      <c r="D27" s="31" t="s">
+        <v>224</v>
+      </c>
+      <c r="E27" s="16">
+        <v>1</v>
+      </c>
+      <c r="F27" s="16">
+        <v>101.15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="17" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3304,10 +3566,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -3369,7 +3631,7 @@
         <v>2.19</v>
       </c>
       <c r="G2">
-        <f t="shared" ref="G2:G8" si="0">E2*F2</f>
+        <f t="shared" ref="G2:G9" si="0">E2*F2</f>
         <v>2.19</v>
       </c>
       <c r="I2" t="s">
@@ -3531,6 +3793,27 @@
       </c>
       <c r="H8" t="s">
         <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>214</v>
+      </c>
+      <c r="B9" t="s">
+        <v>216</v>
+      </c>
+      <c r="D9" t="s">
+        <v>215</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>290.20999999999998</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>290.20999999999998</v>
       </c>
     </row>
   </sheetData>
@@ -3708,7 +3991,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added male receptacles for USB and I2C
</commit_message>
<xml_diff>
--- a/BOM/BOM_Master_2018.xlsx
+++ b/BOM/BOM_Master_2018.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\codyb\USST\rover-hardware\BOM\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44719051-88A3-408C-889A-EED9CB67F8EA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="525" windowWidth="37785" windowHeight="15930" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="530" windowWidth="37790" windowHeight="15930" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Total Cost" sheetId="1" r:id="rId1"/>
@@ -21,12 +27,19 @@
     <sheet name="Antenna" sheetId="13" r:id="rId12"/>
     <sheet name="Misc" sheetId="12" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="179021"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="229">
   <si>
     <t>Manufacturer No.</t>
   </si>
@@ -731,12 +744,21 @@
   <si>
     <t>TemCo Industrial</t>
   </si>
+  <si>
+    <t>NC3MAV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XLR Connectors 3C MALE PCB </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
+  </numFmts>
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -853,8 +875,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -864,6 +892,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -890,7 +930,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -955,6 +995,20 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1016,7 +1070,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1049,9 +1103,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1084,6 +1155,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1259,27 +1347,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="50.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" customWidth="1"/>
-    <col min="11" max="11" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.28515625" customWidth="1"/>
-    <col min="13" max="13" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7265625" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.453125" customWidth="1"/>
+    <col min="11" max="11" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.26953125" customWidth="1"/>
+    <col min="13" max="13" width="14.81640625" customWidth="1"/>
     <col min="14" max="14" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30">
+    <row r="1" spans="1:4">
       <c r="B1" s="8" t="s">
         <v>104</v>
       </c>
@@ -1575,16 +1663,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="5" max="5" width="56.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -1641,7 +1729,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="25.5">
+    <row r="4" spans="1:9" ht="25">
       <c r="A4" s="1" t="s">
         <v>129</v>
       </c>
@@ -1668,7 +1756,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="25.5">
+    <row r="5" spans="1:9" ht="25">
       <c r="A5" s="22" t="s">
         <v>134</v>
       </c>
@@ -1696,7 +1784,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="25.5">
+    <row r="6" spans="1:9" ht="25">
       <c r="A6" s="1" t="s">
         <v>136</v>
       </c>
@@ -1777,19 +1865,19 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1815,7 +1903,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="25.5">
+    <row r="2" spans="1:7" ht="25">
       <c r="A2" s="1" t="s">
         <v>151</v>
       </c>
@@ -1850,17 +1938,17 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="90.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.453125" customWidth="1"/>
+    <col min="4" max="4" width="90.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1983,16 +2071,16 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2048,17 +2136,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="4" max="4" width="60.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="60.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -2118,7 +2206,7 @@
         <v>13.9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75">
+    <row r="3" spans="1:10" ht="15.5">
       <c r="A3" s="27" t="s">
         <v>176</v>
       </c>
@@ -2169,7 +2257,7 @@
         <v>17.309999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75">
+    <row r="5" spans="1:10" ht="15.5">
       <c r="A5" s="27" t="s">
         <v>186</v>
       </c>
@@ -2183,7 +2271,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75">
+    <row r="6" spans="1:10" ht="15.5">
       <c r="A6" s="27" t="s">
         <v>183</v>
       </c>
@@ -2536,7 +2624,7 @@
         <v>70</v>
       </c>
       <c r="G20">
-        <f t="shared" ref="G20:G24" si="1">E20*F20</f>
+        <f t="shared" ref="G20:G22" si="1">E20*F20</f>
         <v>70</v>
       </c>
     </row>
@@ -2592,7 +2680,7 @@
       <c r="A23" s="1"/>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="1:8" ht="22.5">
+    <row r="24" spans="1:8" ht="23">
       <c r="A24" s="29" t="s">
         <v>217</v>
       </c>
@@ -2606,7 +2694,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="22.5">
+    <row r="25" spans="1:8" ht="23">
       <c r="A25" s="29" t="s">
         <v>221</v>
       </c>
@@ -2617,7 +2705,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="33.75">
+    <row r="26" spans="1:8" ht="34.5">
       <c r="A26" s="29" t="s">
         <v>222</v>
       </c>
@@ -2653,17 +2741,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="4" max="4" width="60.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="60.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -2747,7 +2835,7 @@
         <v>11.59</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75">
+    <row r="4" spans="1:10" ht="15.5">
       <c r="A4" s="27" t="s">
         <v>180</v>
       </c>
@@ -2983,19 +3071,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7265625" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -3249,7 +3337,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="45">
+    <row r="14" spans="1:10" ht="43.5">
       <c r="A14" s="18" t="s">
         <v>142</v>
       </c>
@@ -3301,7 +3389,7 @@
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" spans="1:10" ht="45">
+    <row r="16" spans="1:10" ht="29">
       <c r="A16" s="18" t="s">
         <v>146</v>
       </c>
@@ -3360,26 +3448,26 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A15" r:id="rId1" display="https://www.molex.com/molex/products/datasheet.jsp?part=active/0002061131_CRIMP_TERMINALS.xml"/>
-    <hyperlink ref="A17" r:id="rId2" display="https://www.molex.com/molex/products/datasheet.jsp?part=active/0002062101_CRIMP_TERMINALS.xml"/>
+    <hyperlink ref="A15" r:id="rId1" display="https://www.molex.com/molex/products/datasheet.jsp?part=active/0002061131_CRIMP_TERMINALS.xml" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="A17" r:id="rId2" display="https://www.molex.com/molex/products/datasheet.jsp?part=active/0002062101_CRIMP_TERMINALS.xml" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="50.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -3565,17 +3653,17 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -3818,7 +3906,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A6" r:id="rId1" display="https://www.mouser.ca/ProductDetail/Adafruit/3445?qs=sGAEpiMZZMu%252bmKbOcEVhFQxTf6VNDqZlHHxJgTmlxQIH1iVmUF7%252bAg%3d%3d"/>
+    <hyperlink ref="A6" r:id="rId1" display="https://www.mouser.ca/ProductDetail/Adafruit/3445?qs=sGAEpiMZZMu%252bmKbOcEVhFQxTf6VNDqZlHHxJgTmlxQIH1iVmUF7%252bAg%3d%3d" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="17" orientation="portrait" verticalDpi="0" r:id="rId2"/>
@@ -3826,16 +3914,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:G8"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="4" max="4" width="79.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="79.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -3876,7 +3964,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="30">
+    <row r="3" spans="1:10" ht="29">
       <c r="A3" s="6" t="s">
         <v>77</v>
       </c>
@@ -3927,7 +4015,7 @@
         <v>2.62</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="30">
+    <row r="6" spans="1:10" ht="29">
       <c r="A6" s="6" t="s">
         <v>80</v>
       </c>
@@ -3951,53 +4039,73 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="30">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:10" ht="29">
+      <c r="A7" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="5" t="s">
+      <c r="C7" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="E7" s="5">
-        <v>1</v>
-      </c>
-      <c r="F7" s="5">
+      <c r="E7" s="33">
+        <v>1</v>
+      </c>
+      <c r="F7" s="33">
         <v>13.73</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="33">
         <f>E7*F7</f>
         <v>13.73</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="9"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
+      <c r="A8" s="37" t="s">
+        <v>227</v>
+      </c>
+      <c r="B8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="34" t="s">
+        <v>228</v>
+      </c>
+      <c r="E8" s="5">
+        <v>1</v>
+      </c>
+      <c r="F8" s="35">
+        <v>1.71</v>
+      </c>
+      <c r="G8" s="5">
+        <v>1.71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="D9" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="4" max="4" width="79.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="79.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -4031,7 +4139,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="38.25">
+    <row r="3" spans="1:8" ht="37.5">
       <c r="A3" s="1" t="s">
         <v>198</v>
       </c>
@@ -4055,7 +4163,7 @@
         <v>12.82</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="25.5">
+    <row r="4" spans="1:8" ht="25">
       <c r="A4" s="1" t="s">
         <v>202</v>
       </c>
@@ -4079,7 +4187,7 @@
         <v>15.07</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1"/>
+    <row r="8" spans="1:8" ht="15" thickBot="1"/>
     <row r="9" spans="1:8">
       <c r="A9" s="11"/>
     </row>
@@ -4090,16 +4198,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="A10:C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="4" max="4" width="79.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="79.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -4229,7 +4337,7 @@
         <v>3.49</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1">
+    <row r="8" spans="1:8" ht="15" thickBot="1">
       <c r="A8" t="s">
         <v>51</v>
       </c>

</xml_diff>